<commit_message>
Manage course link addition is done
</commit_message>
<xml_diff>
--- a/timetablescheduler/Settings/student.xlsx
+++ b/timetablescheduler/Settings/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Chandrika\FE\gitHub\Personal\Smart_Class_Crew\timetablescheduler\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA64E76-C9ED-4208-AF21-D8C671FEF3DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6C73FD-77C9-4066-8970-4963090EE364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{F12E7B74-3F02-4A01-96CC-3AB15A1310FF}"/>
   </bookViews>
@@ -25,39 +25,123 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>sl_no</t>
   </si>
   <si>
+    <t>usn</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
-    <t>usn</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>divison</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Chandrika</t>
-  </si>
-  <si>
-    <t>01FS24BEC013</t>
-  </si>
-  <si>
-    <t>01FS24BEC013@kletech.ac.in</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>female</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>01FS24BEC015</t>
+  </si>
+  <si>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>CDE</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>EFG</t>
+  </si>
+  <si>
+    <t>FGH</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>IJK</t>
+  </si>
+  <si>
+    <t>HIJ</t>
+  </si>
+  <si>
+    <t>JKL</t>
+  </si>
+  <si>
+    <t>01FS24BEC016</t>
+  </si>
+  <si>
+    <t>01FS24BEC017</t>
+  </si>
+  <si>
+    <t>01FS24BEC018</t>
+  </si>
+  <si>
+    <t>01FS24BEC019</t>
+  </si>
+  <si>
+    <t>01FS24BEC020</t>
+  </si>
+  <si>
+    <t>01FS24BEC021</t>
+  </si>
+  <si>
+    <t>01FS24BEC022</t>
+  </si>
+  <si>
+    <t>01FS24BEC023</t>
+  </si>
+  <si>
+    <t>01FS24BEC024</t>
+  </si>
+  <si>
+    <t>01FS24BEC017@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC018@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC019@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC020@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC021@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC022@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC023@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC024@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC025@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>01FS24BEC026@kletech.ac.in</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -420,15 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89DD32D-41C3-4399-B6D6-83D44234AA95}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.36328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -438,19 +522,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -458,24 +542,213 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{D4931142-B4F6-4D68-874E-EE259F6C179A}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{CD19E3BD-25DB-4934-ADCE-311B6B9B4507}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{F930941E-5365-4491-8176-9305A8881EE4}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{326C5874-9D4A-49B4-AE73-59E04262E4D6}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{799C23F5-C816-4DCC-A94A-11A0E50E0FA1}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{8B244C18-49C1-46A0-A68E-38DDC2C9B509}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{4AD25074-295D-438A-8593-839D070C0A6E}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{0B285D8A-0725-4AEF-8772-861E500B25E9}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{C78583C7-9CF8-4C28-BD02-A352604C6DB4}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{35BA4C88-E5CB-49E0-8B16-54C4503282C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>